<commit_message>
Version 1.2.3 UI Improvements
</commit_message>
<xml_diff>
--- a/docs/V20 MODBUS RS485 .xlsx
+++ b/docs/V20 MODBUS RS485 .xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tstechnologies-my.sharepoint.com/personal/gary_twinn_net/Documents/GTFiles/PhD/Python Projects/UCL-tombola/Manuals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tstechnologies-my.sharepoint.com/personal/gary_twinn_net/Documents/GTFiles/PhD/Python Projects/UCL-tombola/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{4987A5B0-BF6A-4591-8726-1D025222C751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2660FF60-2E39-4D98-BE9C-D4F5CC92A072}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{4987A5B0-BF6A-4591-8726-1D025222C751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{127DF848-D43A-40B1-9F56-80E0BADCE13A}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="0" windowWidth="22500" windowHeight="12680" xr2:uid="{C2114098-FEB7-4AC9-8A53-85B8F6D09A7F}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="22500" windowHeight="14170" xr2:uid="{C2114098-FEB7-4AC9-8A53-85B8F6D09A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="V20" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="256">
+  <si>
+    <t>Converter</t>
+  </si>
+  <si>
+    <t>MODBUS</t>
+  </si>
   <si>
     <t>Description</t>
   </si>
@@ -59,12 +65,6 @@
     <t>Write</t>
   </si>
   <si>
-    <t>Converter</t>
-  </si>
-  <si>
-    <t>MODBUS</t>
-  </si>
-  <si>
     <t>Watchdog time</t>
   </si>
   <si>
@@ -95,6 +95,9 @@
     <t>HSW</t>
   </si>
   <si>
+    <t>Command</t>
+  </si>
+  <si>
     <t>Run enable</t>
   </si>
   <si>
@@ -257,6 +260,9 @@
     <t>P2265</t>
   </si>
   <si>
+    <t>jog1</t>
+  </si>
+  <si>
     <t>Frequency output</t>
   </si>
   <si>
@@ -266,6 +272,9 @@
     <t>r0024</t>
   </si>
   <si>
+    <t>Query</t>
+  </si>
+  <si>
     <t>Speed</t>
   </si>
   <si>
@@ -795,15 +804,6 @@
   </si>
   <si>
     <t>DS47 data 120</t>
-  </si>
-  <si>
-    <t>Command</t>
-  </si>
-  <si>
-    <t>Query</t>
-  </si>
-  <si>
-    <t>jog1</t>
   </si>
 </sst>
 </file>
@@ -879,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -898,7 +898,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -914,6 +913,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1213,13 +1216,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B285474-0D1C-4231-8E00-803C94ED280B}">
-  <dimension ref="A1:P148"/>
+  <dimension ref="A1:O148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:D40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="11.81640625" style="1" customWidth="1"/>
@@ -1229,7 +1232,7 @@
     <col min="7" max="7" width="8.7265625" style="1"/>
     <col min="8" max="8" width="14.26953125" style="1" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="14.08984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1796875" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.7265625" style="1"/>
     <col min="12" max="12" width="19.54296875" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.54296875" style="1" customWidth="1"/>
@@ -1238,32 +1241,32 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1357,7 +1360,7 @@
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="M4" s="1">
         <v>50</v>
@@ -1371,7 +1374,7 @@
         <v>40004</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1383,18 +1386,18 @@
         <v>1</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="5" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="M5" s="1">
         <v>1</v>
@@ -1408,7 +1411,7 @@
         <v>40005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>10</v>
@@ -1420,18 +1423,18 @@
         <v>1</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
@@ -1445,7 +1448,7 @@
         <v>40006</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>10</v>
@@ -1457,18 +1460,18 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="5" t="s">
-        <v>253</v>
+        <v>19</v>
       </c>
       <c r="M7" s="1">
         <v>1</v>
@@ -1482,7 +1485,7 @@
         <v>40007</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -1494,14 +1497,14 @@
         <v>1</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1512,7 +1515,7 @@
         <v>40008</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -1529,10 +1532,10 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1543,7 +1546,7 @@
         <v>40009</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>10</v>
@@ -1555,14 +1558,14 @@
         <v>1</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1573,7 +1576,7 @@
         <v>40010</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
@@ -1585,14 +1588,14 @@
         <v>10</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1603,26 +1606,26 @@
         <v>40011</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3">
         <v>100</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1633,26 +1636,26 @@
         <v>40012</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3">
         <v>100</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1663,7 +1666,7 @@
         <v>40013</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1681,7 +1684,7 @@
         <v>40014</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>10</v>
@@ -1693,16 +1696,16 @@
         <v>1</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1713,7 +1716,7 @@
         <v>40015</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>10</v>
@@ -1725,16 +1728,16 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -1745,26 +1748,26 @@
         <v>40016</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F17" s="3">
         <v>100</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H17" s="6"/>
       <c r="I17" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -1775,7 +1778,7 @@
         <v>40017</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>10</v>
@@ -1792,10 +1795,10 @@
       </c>
       <c r="H18" s="6"/>
       <c r="I18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -1806,7 +1809,7 @@
         <v>40018</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>10</v>
@@ -1823,10 +1826,10 @@
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1837,7 +1840,7 @@
         <v>40019</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>10</v>
@@ -1849,14 +1852,14 @@
         <v>1000</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1867,26 +1870,26 @@
         <v>40020</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1897,7 +1900,7 @@
         <v>40021</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>10</v>
@@ -1909,14 +1912,14 @@
         <v>1</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H22" s="6"/>
       <c r="I22" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -1927,7 +1930,7 @@
         <v>40022</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>10</v>
@@ -1939,14 +1942,14 @@
         <v>100</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -1957,7 +1960,7 @@
         <v>40023</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>10</v>
@@ -1969,17 +1972,17 @@
         <v>100</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>255</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -1990,13 +1993,13 @@
         <v>40024</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F25" s="4">
         <v>100</v>
@@ -2007,14 +2010,17 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K25" s="5"/>
       <c r="L25" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
       </c>
       <c r="N25" s="1">
         <v>0</v>
@@ -2031,13 +2037,13 @@
         <v>40025</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F26" s="4">
         <v>1</v>
@@ -2048,14 +2054,17 @@
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K26" s="5"/>
       <c r="L26" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
@@ -2072,30 +2081,33 @@
         <v>40026</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F27" s="4">
         <v>100</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M27" s="1">
+        <v>2</v>
       </c>
       <c r="N27" s="1">
         <v>0</v>
@@ -2112,13 +2124,13 @@
         <v>40027</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F28" s="4">
         <v>100</v>
@@ -2129,14 +2141,17 @@
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M28" s="1">
+        <v>3</v>
       </c>
       <c r="N28" s="1">
         <v>0</v>
@@ -2153,30 +2168,33 @@
         <v>40028</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F29" s="4">
         <v>100</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K29" s="5"/>
       <c r="L29" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M29" s="1">
+        <v>4</v>
       </c>
       <c r="N29" s="1">
         <v>0</v>
@@ -2193,30 +2211,33 @@
         <v>40029</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F30" s="4">
         <v>1</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K30" s="5"/>
       <c r="L30" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M30" s="1">
+        <v>5</v>
       </c>
       <c r="N30" s="1">
         <v>0</v>
@@ -2233,30 +2254,33 @@
         <v>40030</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F31" s="4">
-        <v>1</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K31" s="5"/>
       <c r="L31" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M31" s="1">
+        <v>6</v>
       </c>
       <c r="N31" s="1">
         <v>326</v>
@@ -2273,13 +2297,13 @@
         <v>40031</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F32" s="4">
         <v>100</v>
@@ -2290,14 +2314,17 @@
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M32" s="1">
+        <v>7</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
@@ -2306,7 +2333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2314,30 +2341,33 @@
         <v>40032</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F33" s="4">
         <v>100</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="K33" s="5"/>
       <c r="L33" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M33" s="1">
+        <v>8</v>
       </c>
       <c r="N33" s="1">
         <v>37</v>
@@ -2346,7 +2376,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2354,30 +2384,33 @@
         <v>40033</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="F34" s="4">
-        <v>1</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="K34" s="5"/>
       <c r="L34" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M34" s="1">
+        <v>9</v>
       </c>
       <c r="N34" s="1">
         <v>0</v>
@@ -2386,7 +2419,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>33</v>
       </c>
@@ -2394,10 +2427,10 @@
         <v>40034</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>13</v>
@@ -2406,20 +2439,23 @@
         <v>1</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M35" s="1">
+        <v>10</v>
       </c>
       <c r="N35" s="1">
         <v>1</v>
@@ -2428,7 +2464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2436,10 +2472,10 @@
         <v>40035</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>13</v>
@@ -2448,20 +2484,23 @@
         <v>1</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M36" s="1">
+        <v>11</v>
       </c>
       <c r="N36" s="1">
         <v>0</v>
@@ -2470,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2478,10 +2517,10 @@
         <v>40036</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>13</v>
@@ -2490,20 +2529,23 @@
         <v>1</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M37" s="1">
+        <v>12</v>
       </c>
       <c r="N37" s="1">
         <v>0</v>
@@ -2512,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2520,10 +2562,10 @@
         <v>40037</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>13</v>
@@ -2532,31 +2574,32 @@
         <v>1</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8">
-        <v>1</v>
-      </c>
-      <c r="O38" s="8">
-        <v>1</v>
-      </c>
-      <c r="P38" s="8"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="M38" s="1">
+        <v>13</v>
+      </c>
+      <c r="N38" s="1">
+        <v>1</v>
+      </c>
+      <c r="O38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -2564,10 +2607,10 @@
         <v>40038</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>13</v>
@@ -2576,20 +2619,23 @@
         <v>1</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K39" s="5"/>
       <c r="L39" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M39" s="1">
+        <v>14</v>
       </c>
       <c r="N39" s="1">
         <v>1</v>
@@ -2598,7 +2644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -2606,10 +2652,10 @@
         <v>40039</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>13</v>
@@ -2618,20 +2664,23 @@
         <v>1</v>
       </c>
       <c r="G40" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H40" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="H40" s="4" t="s">
-        <v>121</v>
-      </c>
       <c r="I40" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5" t="s">
-        <v>254</v>
+        <v>78</v>
+      </c>
+      <c r="M40" s="1">
+        <v>15</v>
       </c>
       <c r="N40" s="1">
         <v>0</v>
@@ -2640,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2648,10 +2697,10 @@
         <v>40040</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>16</v>
@@ -2665,13 +2714,13 @@
       </c>
       <c r="H41" s="6"/>
       <c r="I41" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -2679,10 +2728,10 @@
         <v>40041</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>16</v>
@@ -2696,13 +2745,13 @@
       </c>
       <c r="H42" s="6"/>
       <c r="I42" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2710,10 +2759,10 @@
         <v>40042</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>16</v>
@@ -2727,13 +2776,13 @@
       </c>
       <c r="H43" s="6"/>
       <c r="I43" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -2741,10 +2790,10 @@
         <v>40044</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>16</v>
@@ -2758,13 +2807,13 @@
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -2772,10 +2821,10 @@
         <v>40045</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>16</v>
@@ -2789,13 +2838,13 @@
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -2803,10 +2852,10 @@
         <v>40046</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>16</v>
@@ -2820,13 +2869,13 @@
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -2834,10 +2883,10 @@
         <v>40047</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>16</v>
@@ -2851,13 +2900,13 @@
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -2865,10 +2914,10 @@
         <v>40048</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>13</v>
@@ -2877,19 +2926,19 @@
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -2897,10 +2946,10 @@
         <v>40049</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>13</v>
@@ -2909,19 +2958,19 @@
         <v>1</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -2929,10 +2978,10 @@
         <v>40050</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>13</v>
@@ -2941,19 +2990,19 @@
         <v>1</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -2961,10 +3010,10 @@
         <v>40051</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>13</v>
@@ -2973,19 +3022,19 @@
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>53</v>
       </c>
@@ -2993,10 +3042,10 @@
         <v>40054</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>13</v>
@@ -3005,19 +3054,19 @@
         <v>1</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>54</v>
       </c>
@@ -3025,10 +3074,10 @@
         <v>40055</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>13</v>
@@ -3037,17 +3086,17 @@
         <v>1</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>55</v>
       </c>
@@ -3055,10 +3104,10 @@
         <v>40056</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>13</v>
@@ -3067,17 +3116,17 @@
         <v>1</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>56</v>
       </c>
@@ -3085,10 +3134,10 @@
         <v>40057</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>13</v>
@@ -3097,17 +3146,17 @@
         <v>1</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>57</v>
       </c>
@@ -3115,10 +3164,10 @@
         <v>40058</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>13</v>
@@ -3127,17 +3176,17 @@
         <v>1</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>58</v>
       </c>
@@ -3145,10 +3194,10 @@
         <v>40059</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>13</v>
@@ -3157,19 +3206,19 @@
         <v>1</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>59</v>
       </c>
@@ -3177,10 +3226,10 @@
         <v>40060</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>13</v>
@@ -3189,17 +3238,17 @@
         <v>1</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H58" s="6"/>
       <c r="I58" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>60</v>
       </c>
@@ -3207,10 +3256,10 @@
         <v>40061</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>13</v>
@@ -3219,17 +3268,17 @@
         <v>100</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H59" s="6"/>
       <c r="I59" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>61</v>
       </c>
@@ -3237,10 +3286,10 @@
         <v>40062</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>13</v>
@@ -3249,45 +3298,49 @@
         <v>1</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61" s="3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="4">
         <v>99</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="4">
         <v>40100</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F61" s="3">
-        <v>1</v>
-      </c>
-      <c r="G61" s="6"/>
-      <c r="H61" s="6"/>
-      <c r="I61" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C61" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>100</v>
       </c>
@@ -3309,13 +3362,13 @@
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>109</v>
       </c>
@@ -3323,10 +3376,10 @@
         <v>40110</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>13</v>
@@ -3337,13 +3390,13 @@
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
       <c r="I63" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>110</v>
       </c>
@@ -3351,10 +3404,10 @@
         <v>40111</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>13</v>
@@ -3365,10 +3418,10 @@
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
       <c r="I64" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -3379,7 +3432,7 @@
         <v>40200</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>10</v>
@@ -3391,16 +3444,16 @@
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -3411,7 +3464,7 @@
         <v>40201</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>10</v>
@@ -3423,16 +3476,16 @@
         <v>1</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
@@ -3443,7 +3496,7 @@
         <v>40202</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>10</v>
@@ -3455,16 +3508,16 @@
         <v>1</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
@@ -3475,7 +3528,7 @@
         <v>40203</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>10</v>
@@ -3487,16 +3540,16 @@
         <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I68" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J68" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
@@ -3507,10 +3560,10 @@
         <v>40220</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>16</v>
@@ -3524,10 +3577,10 @@
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
@@ -3538,10 +3591,10 @@
         <v>40240</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>13</v>
@@ -3550,16 +3603,16 @@
         <v>1</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
@@ -3570,10 +3623,10 @@
         <v>40241</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>13</v>
@@ -3582,16 +3635,16 @@
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
@@ -3602,10 +3655,10 @@
         <v>40242</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>13</v>
@@ -3614,16 +3667,16 @@
         <v>1</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -3634,10 +3687,10 @@
         <v>40243</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>13</v>
@@ -3646,16 +3699,16 @@
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -3666,10 +3719,10 @@
         <v>40244</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>13</v>
@@ -3678,16 +3731,16 @@
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -3698,10 +3751,10 @@
         <v>40245</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E75" s="3" t="s">
         <v>13</v>
@@ -3710,16 +3763,16 @@
         <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="J75" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -3730,10 +3783,10 @@
         <v>40260</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>16</v>
@@ -3747,10 +3800,10 @@
       </c>
       <c r="H76" s="6"/>
       <c r="I76" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J76" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -3761,10 +3814,10 @@
         <v>40261</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>16</v>
@@ -3778,10 +3831,10 @@
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -3792,10 +3845,10 @@
         <v>40300</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>13</v>
@@ -3804,14 +3857,14 @@
         <v>1</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H78" s="6"/>
       <c r="I78" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="J78" s="3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -3822,10 +3875,10 @@
         <v>40301</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>13</v>
@@ -3834,14 +3887,14 @@
         <v>100</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H79" s="6"/>
       <c r="I79" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J79" s="3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -3852,26 +3905,26 @@
         <v>40320</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F80" s="3">
         <v>100</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H80" s="6"/>
       <c r="I80" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J80" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
@@ -3882,7 +3935,7 @@
         <v>40321</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>10</v>
@@ -3894,14 +3947,14 @@
         <v>10</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
@@ -3912,26 +3965,26 @@
         <v>40322</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F82" s="3">
         <v>100</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
@@ -3942,26 +3995,26 @@
         <v>40323</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F83" s="3">
         <v>100</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J83" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
@@ -3972,26 +4025,26 @@
         <v>40324</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F84" s="3">
         <v>100</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H84" s="6"/>
       <c r="I84" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
@@ -4002,13 +4055,13 @@
         <v>40325</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F85" s="3">
         <v>100</v>
@@ -4019,10 +4072,10 @@
       </c>
       <c r="H85" s="6"/>
       <c r="I85" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="J85" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -4033,13 +4086,13 @@
         <v>40326</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F86" s="3">
         <v>100</v>
@@ -4050,10 +4103,10 @@
       </c>
       <c r="H86" s="6"/>
       <c r="I86" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
@@ -4064,13 +4117,13 @@
         <v>40327</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F87" s="3">
         <v>100</v>
@@ -4081,10 +4134,10 @@
       </c>
       <c r="H87" s="6"/>
       <c r="I87" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -4095,13 +4148,13 @@
         <v>40328</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F88" s="3">
         <v>100</v>
@@ -4112,10 +4165,10 @@
       </c>
       <c r="H88" s="6"/>
       <c r="I88" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -4126,7 +4179,7 @@
         <v>40330</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>10</v>
@@ -4143,10 +4196,10 @@
       </c>
       <c r="H89" s="6"/>
       <c r="I89" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
@@ -4157,7 +4210,7 @@
         <v>40331</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>10</v>
@@ -4174,10 +4227,10 @@
       </c>
       <c r="H90" s="6"/>
       <c r="I90" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -4188,13 +4241,13 @@
         <v>40332</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F91" s="3">
         <v>100</v>
@@ -4205,10 +4258,10 @@
       </c>
       <c r="H91" s="6"/>
       <c r="I91" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="J91" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
@@ -4219,13 +4272,13 @@
         <v>40333</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F92" s="3">
         <v>100</v>
@@ -4236,10 +4289,10 @@
       </c>
       <c r="H92" s="6"/>
       <c r="I92" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="J92" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
@@ -4250,13 +4303,13 @@
         <v>40334</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F93" s="3">
         <v>100</v>
@@ -4267,10 +4320,10 @@
       </c>
       <c r="H93" s="6"/>
       <c r="I93" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="J93" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.3">
@@ -4281,13 +4334,13 @@
         <v>40335</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F94" s="3">
         <v>100</v>
@@ -4298,10 +4351,10 @@
       </c>
       <c r="H94" s="6"/>
       <c r="I94" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="J94" s="3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
@@ -4312,13 +4365,13 @@
         <v>40340</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F95" s="3">
         <v>100</v>
@@ -4329,10 +4382,10 @@
       </c>
       <c r="H95" s="6"/>
       <c r="I95" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J95" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
@@ -4343,13 +4396,13 @@
         <v>40341</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F96" s="3">
         <v>1</v>
@@ -4360,10 +4413,10 @@
       </c>
       <c r="H96" s="6"/>
       <c r="I96" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="J96" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.3">
@@ -4374,13 +4427,13 @@
         <v>40342</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F97" s="3">
         <v>100</v>
@@ -4391,10 +4444,10 @@
       </c>
       <c r="H97" s="6"/>
       <c r="I97" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J97" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.3">
@@ -4405,26 +4458,26 @@
         <v>40343</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E98" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F98" s="3">
+        <v>1</v>
+      </c>
+      <c r="G98" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="F98" s="3">
-        <v>1</v>
-      </c>
-      <c r="G98" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="H98" s="6"/>
       <c r="I98" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.3">
@@ -4435,26 +4488,26 @@
         <v>40344</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E99" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F99" s="3">
+        <v>1</v>
+      </c>
+      <c r="G99" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="F99" s="3">
-        <v>1</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="H99" s="6"/>
       <c r="I99" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.3">
@@ -4465,26 +4518,26 @@
         <v>40345</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F100" s="3">
         <v>100</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H100" s="6"/>
       <c r="I100" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="J100" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.3">
@@ -4495,13 +4548,13 @@
         <v>40346</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F101" s="3">
         <v>100</v>
@@ -4512,10 +4565,10 @@
       </c>
       <c r="H101" s="6"/>
       <c r="I101" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="J101" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.3">
@@ -4526,26 +4579,26 @@
         <v>40347</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F102" s="3">
         <v>100</v>
       </c>
       <c r="G102" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H102" s="6"/>
       <c r="I102" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.3">
@@ -4556,26 +4609,26 @@
         <v>40348</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F103" s="3">
         <v>1</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H103" s="6"/>
       <c r="I103" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="J103" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.3">
@@ -4586,10 +4639,10 @@
         <v>40349</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>13</v>
@@ -4598,16 +4651,16 @@
         <v>1</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="H104" s="3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
@@ -4618,26 +4671,26 @@
         <v>40350</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F105" s="3">
         <v>100</v>
       </c>
       <c r="G105" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H105" s="6"/>
       <c r="I105" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J105" s="3" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.3">
@@ -4648,7 +4701,7 @@
         <v>40360</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>10</v>
@@ -4660,14 +4713,14 @@
         <v>10</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H106" s="6"/>
       <c r="I106" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.3">
@@ -4678,26 +4731,26 @@
         <v>40361</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D107" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F107" s="3">
         <v>100</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H107" s="6"/>
       <c r="I107" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.3">
@@ -4708,26 +4761,26 @@
         <v>40362</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D108" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F108" s="3">
         <v>100</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H108" s="6"/>
       <c r="I108" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J108" s="3" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.3">
@@ -4738,26 +4791,26 @@
         <v>40369</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F109" s="3">
         <v>100</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H109" s="6"/>
       <c r="I109" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="J109" s="3" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
@@ -4768,26 +4821,26 @@
         <v>40370</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D110" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F110" s="3">
         <v>100</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H110" s="6"/>
       <c r="I110" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.3">
@@ -4798,26 +4851,26 @@
         <v>40371</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D111" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F111" s="3">
         <v>100</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H111" s="6"/>
       <c r="I111" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.3">
@@ -4828,26 +4881,26 @@
         <v>40372</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D112" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F112" s="3">
         <v>100</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H112" s="6"/>
       <c r="I112" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.3">
@@ -4858,26 +4911,26 @@
         <v>40373</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D113" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F113" s="3">
         <v>100</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H113" s="6"/>
       <c r="I113" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.3">
@@ -4888,26 +4941,26 @@
         <v>40374</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F114" s="3">
         <v>100</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H114" s="6"/>
       <c r="I114" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="J114" s="3" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.3">
@@ -4918,10 +4971,10 @@
         <v>40400</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E115" s="3" t="s">
         <v>13</v>
@@ -4930,14 +4983,14 @@
         <v>1</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H115" s="6"/>
       <c r="I115" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="J115" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.3">
@@ -4948,10 +5001,10 @@
         <v>40401</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E116" s="3" t="s">
         <v>13</v>
@@ -4960,14 +5013,14 @@
         <v>1</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H116" s="6"/>
       <c r="I116" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.3">
@@ -4978,10 +5031,10 @@
         <v>40402</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E117" s="3" t="s">
         <v>13</v>
@@ -4990,14 +5043,14 @@
         <v>1</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H117" s="6"/>
       <c r="I117" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J117" s="3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.3">
@@ -5008,10 +5061,10 @@
         <v>40403</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E118" s="3" t="s">
         <v>13</v>
@@ -5020,14 +5073,14 @@
         <v>1</v>
       </c>
       <c r="G118" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H118" s="6"/>
       <c r="I118" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="J118" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
@@ -5038,10 +5091,10 @@
         <v>40404</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E119" s="3" t="s">
         <v>13</v>
@@ -5050,14 +5103,14 @@
         <v>1</v>
       </c>
       <c r="G119" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H119" s="6"/>
       <c r="I119" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
@@ -5068,10 +5121,10 @@
         <v>40405</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E120" s="3" t="s">
         <v>13</v>
@@ -5080,14 +5133,14 @@
         <v>1</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H120" s="6"/>
       <c r="I120" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
@@ -5098,10 +5151,10 @@
         <v>40406</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E121" s="3" t="s">
         <v>13</v>
@@ -5110,14 +5163,14 @@
         <v>1</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H121" s="6"/>
       <c r="I121" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
@@ -5128,10 +5181,10 @@
         <v>40407</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E122" s="3" t="s">
         <v>13</v>
@@ -5140,14 +5193,14 @@
         <v>1</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H122" s="6"/>
       <c r="I122" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="J122" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
@@ -5158,10 +5211,10 @@
         <v>40408</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E123" s="3" t="s">
         <v>13</v>
@@ -5170,14 +5223,14 @@
         <v>1</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H123" s="6"/>
       <c r="I123" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="J123" s="3" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
@@ -5188,10 +5241,10 @@
         <v>40499</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E124" s="3" t="s">
         <v>13</v>
@@ -5200,7 +5253,7 @@
         <v>1</v>
       </c>
       <c r="G124" s="6" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H124" s="6"/>
       <c r="I124" s="3" t="s">
@@ -5218,7 +5271,7 @@
         <v>40500</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>10</v>
@@ -5230,14 +5283,14 @@
         <v>1</v>
       </c>
       <c r="G125" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H125" s="6"/>
       <c r="I125" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J125" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.3">
@@ -5248,7 +5301,7 @@
         <v>40501</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>10</v>
@@ -5265,10 +5318,10 @@
       </c>
       <c r="H126" s="6"/>
       <c r="I126" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J126" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.3">
@@ -5279,7 +5332,7 @@
         <v>40510</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>10</v>
@@ -5291,14 +5344,14 @@
         <v>100</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="H127" s="6"/>
       <c r="I127" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J127" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.3">
@@ -5309,7 +5362,7 @@
         <v>40511</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>10</v>
@@ -5321,14 +5374,14 @@
         <v>100</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H128" s="6"/>
       <c r="I128" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J128" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.3">
@@ -5339,7 +5392,7 @@
         <v>40512</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>10</v>
@@ -5351,14 +5404,14 @@
         <v>1000</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H129" s="6"/>
       <c r="I129" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J129" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.3">
@@ -5369,26 +5422,26 @@
         <v>40513</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D130" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F130" s="3">
         <v>1</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H130" s="6"/>
       <c r="I130" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J130" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.3">
@@ -5399,7 +5452,7 @@
         <v>40514</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>10</v>
@@ -5411,14 +5464,14 @@
         <v>1</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H131" s="6"/>
       <c r="I131" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J131" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.3">
@@ -5429,7 +5482,7 @@
         <v>40515</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>10</v>
@@ -5446,10 +5499,10 @@
       </c>
       <c r="H132" s="6"/>
       <c r="I132" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.3">
@@ -5460,7 +5513,7 @@
         <v>40516</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>10</v>
@@ -5477,10 +5530,10 @@
       </c>
       <c r="H133" s="6"/>
       <c r="I133" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.3">
@@ -5491,10 +5544,10 @@
         <v>40520</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E134" s="3" t="s">
         <v>16</v>
@@ -5508,10 +5561,10 @@
       </c>
       <c r="H134" s="6"/>
       <c r="I134" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.3">
@@ -5522,10 +5575,10 @@
         <v>40521</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>16</v>
@@ -5539,10 +5592,10 @@
       </c>
       <c r="H135" s="6"/>
       <c r="I135" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J135" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.3">
@@ -5553,10 +5606,10 @@
         <v>40522</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E136" s="3" t="s">
         <v>16</v>
@@ -5570,10 +5623,10 @@
       </c>
       <c r="H136" s="6"/>
       <c r="I136" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="J136" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.3">
@@ -5584,10 +5637,10 @@
         <v>40550</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E137" s="3" t="s">
         <v>13</v>
@@ -5614,10 +5667,10 @@
         <v>40551</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>13</v>
@@ -5644,10 +5697,10 @@
         <v>40552</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E139" s="3" t="s">
         <v>13</v>
@@ -5674,10 +5727,10 @@
         <v>40554</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E140" s="3" t="s">
         <v>13</v>
@@ -5704,10 +5757,10 @@
         <v>40555</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E141" s="3" t="s">
         <v>13</v>
@@ -5734,10 +5787,10 @@
         <v>40558</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E142" s="3" t="s">
         <v>13</v>
@@ -5764,10 +5817,10 @@
         <v>40559</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>13</v>
@@ -5794,7 +5847,7 @@
         <v>40601</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="D144" s="3" t="s">
         <v>10</v>
@@ -5824,7 +5877,7 @@
         <v>40602</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D145" s="3" t="s">
         <v>10</v>
@@ -5854,7 +5907,7 @@
         <v>40603</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D146" s="3" t="s">
         <v>10</v>
@@ -5878,16 +5931,16 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
@@ -5904,7 +5957,7 @@
         <v>40722</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>10</v>
@@ -5928,34 +5981,88 @@
     </row>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G145:H145"/>
+    <mergeCell ref="G146:H146"/>
+    <mergeCell ref="G147:H147"/>
+    <mergeCell ref="G148:H148"/>
+    <mergeCell ref="G139:H139"/>
+    <mergeCell ref="G140:H140"/>
+    <mergeCell ref="G141:H141"/>
+    <mergeCell ref="G142:H142"/>
+    <mergeCell ref="G143:H143"/>
+    <mergeCell ref="G144:H144"/>
+    <mergeCell ref="G133:H133"/>
+    <mergeCell ref="G134:H134"/>
+    <mergeCell ref="G135:H135"/>
+    <mergeCell ref="G136:H136"/>
+    <mergeCell ref="G137:H137"/>
+    <mergeCell ref="G138:H138"/>
+    <mergeCell ref="G127:H127"/>
+    <mergeCell ref="G128:H128"/>
+    <mergeCell ref="G129:H129"/>
+    <mergeCell ref="G130:H130"/>
+    <mergeCell ref="G131:H131"/>
+    <mergeCell ref="G132:H132"/>
+    <mergeCell ref="G121:H121"/>
+    <mergeCell ref="G122:H122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="G124:H124"/>
+    <mergeCell ref="G125:H125"/>
+    <mergeCell ref="G126:H126"/>
+    <mergeCell ref="G115:H115"/>
+    <mergeCell ref="G116:H116"/>
+    <mergeCell ref="G117:H117"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="G119:H119"/>
+    <mergeCell ref="G120:H120"/>
+    <mergeCell ref="G109:H109"/>
+    <mergeCell ref="G110:H110"/>
+    <mergeCell ref="G111:H111"/>
+    <mergeCell ref="G112:H112"/>
+    <mergeCell ref="G113:H113"/>
+    <mergeCell ref="G114:H114"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="G103:H103"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="G106:H106"/>
+    <mergeCell ref="G107:H107"/>
+    <mergeCell ref="G108:H108"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="G89:H89"/>
+    <mergeCell ref="G78:H78"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="G81:H81"/>
+    <mergeCell ref="G82:H82"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G62:H62"/>
+    <mergeCell ref="G63:H63"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="G76:H76"/>
+    <mergeCell ref="G77:H77"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G58:H58"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G46:H46"/>
@@ -5968,88 +6075,34 @@
     <mergeCell ref="G41:H41"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G62:H62"/>
-    <mergeCell ref="G63:H63"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G76:H76"/>
-    <mergeCell ref="G77:H77"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G58:H58"/>
-    <mergeCell ref="G59:H59"/>
-    <mergeCell ref="G60:H60"/>
-    <mergeCell ref="G61:H61"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="G89:H89"/>
-    <mergeCell ref="G78:H78"/>
-    <mergeCell ref="G79:H79"/>
-    <mergeCell ref="G80:H80"/>
-    <mergeCell ref="G81:H81"/>
-    <mergeCell ref="G82:H82"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="G98:H98"/>
-    <mergeCell ref="G99:H99"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="G109:H109"/>
-    <mergeCell ref="G110:H110"/>
-    <mergeCell ref="G111:H111"/>
-    <mergeCell ref="G112:H112"/>
-    <mergeCell ref="G113:H113"/>
-    <mergeCell ref="G114:H114"/>
-    <mergeCell ref="G102:H102"/>
-    <mergeCell ref="G103:H103"/>
-    <mergeCell ref="G105:H105"/>
-    <mergeCell ref="G106:H106"/>
-    <mergeCell ref="G107:H107"/>
-    <mergeCell ref="G108:H108"/>
-    <mergeCell ref="G121:H121"/>
-    <mergeCell ref="G122:H122"/>
-    <mergeCell ref="G123:H123"/>
-    <mergeCell ref="G124:H124"/>
-    <mergeCell ref="G125:H125"/>
-    <mergeCell ref="G126:H126"/>
-    <mergeCell ref="G115:H115"/>
-    <mergeCell ref="G116:H116"/>
-    <mergeCell ref="G117:H117"/>
-    <mergeCell ref="G118:H118"/>
-    <mergeCell ref="G119:H119"/>
-    <mergeCell ref="G120:H120"/>
-    <mergeCell ref="G133:H133"/>
-    <mergeCell ref="G134:H134"/>
-    <mergeCell ref="G135:H135"/>
-    <mergeCell ref="G136:H136"/>
-    <mergeCell ref="G137:H137"/>
-    <mergeCell ref="G138:H138"/>
-    <mergeCell ref="G127:H127"/>
-    <mergeCell ref="G128:H128"/>
-    <mergeCell ref="G129:H129"/>
-    <mergeCell ref="G130:H130"/>
-    <mergeCell ref="G131:H131"/>
-    <mergeCell ref="G132:H132"/>
-    <mergeCell ref="G145:H145"/>
-    <mergeCell ref="G146:H146"/>
-    <mergeCell ref="G147:H147"/>
-    <mergeCell ref="G148:H148"/>
-    <mergeCell ref="G139:H139"/>
-    <mergeCell ref="G140:H140"/>
-    <mergeCell ref="G141:H141"/>
-    <mergeCell ref="G142:H142"/>
-    <mergeCell ref="G143:H143"/>
-    <mergeCell ref="G144:H144"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>